<commit_message>
import excel-file with inner header
</commit_message>
<xml_diff>
--- a/public/imports/manures.xlsx
+++ b/public/imports/manures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_my_projects\manure\public\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EBEF1F-1C04-4317-8CD8-9BEB39CA4395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1EB45C-FBDD-4F13-A9CE-E3041E8258B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Район 1</t>
   </si>
@@ -61,32 +61,71 @@
     <t>Цель</t>
   </si>
   <si>
-    <t>10 удобрение</t>
-  </si>
-  <si>
-    <t>11 удобрение</t>
-  </si>
-  <si>
-    <t>12 удобрение</t>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Норма азота</t>
+  </si>
+  <si>
+    <t>Норма фосфора</t>
+  </si>
+  <si>
+    <t>Норма калия</t>
+  </si>
+  <si>
+    <t>Культура</t>
+  </si>
+  <si>
+    <t>Район</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Назначение</t>
+  </si>
+  <si>
+    <t>16 удобрение</t>
+  </si>
+  <si>
+    <t>17 удобрение</t>
+  </si>
+  <si>
+    <t>18 удобрение</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAEAEA"/>
+        <bgColor rgb="FFEAEAEA"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -410,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,97 +464,121 @@
     <col min="8" max="9" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="C1" s="1">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="C2" s="1">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>222</v>
+        <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>200</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>540</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -605,6 +669,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>